<commit_message>
Remove WolframAlpha Value columns from four error function spreadsheets
</commit_message>
<xml_diff>
--- a/xlsx/tests/docs/ERF-PRECISE.xlsx
+++ b/xlsx/tests/docs/ERF-PRECISE.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steve\Documents\IronCalc work\IronCalc-clone\IronCalc-SF\xlsx\tests\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF2B7E14-C67E-4562-BFD2-308E4DD41F1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EBDC39C-D512-4767-B293-2BF8EDBBC1A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{BC44EA43-B61B-417F-9ADF-F059B85B51E3}"/>
   </bookViews>
@@ -36,15 +36,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="8">
   <si>
     <t>X</t>
   </si>
   <si>
     <t>Formula Text</t>
-  </si>
-  <si>
-    <t>WolframAlpha Value</t>
   </si>
   <si>
     <t>Formula</t>
@@ -461,7 +458,7 @@
   <dimension ref="A1:D31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32"/>
+      <selection activeCell="D1" sqref="D1:D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -478,14 +475,12 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="D1" s="2"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
@@ -499,9 +494,7 @@
         <f t="shared" ref="C2:C6" ca="1" si="0">_xlfn.FORMULATEXT($B2)</f>
         <v>=ERF.PRECISE($A2)</v>
       </c>
-      <c r="D2" s="3">
-        <v>-0.99999999999846201</v>
-      </c>
+      <c r="D2" s="3"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
@@ -516,9 +509,7 @@
         <f t="shared" ca="1" si="0"/>
         <v>=ERF.PRECISE($A3)</v>
       </c>
-      <c r="D3" s="3">
-        <v>-0.99999999980338306</v>
-      </c>
+      <c r="D3" s="3"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
@@ -533,9 +524,7 @@
         <f t="shared" ca="1" si="0"/>
         <v>=ERF.PRECISE($A4)</v>
       </c>
-      <c r="D4" s="3">
-        <v>-0.99999998458274197</v>
-      </c>
+      <c r="D4" s="3"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
@@ -550,9 +539,7 @@
         <f t="shared" ca="1" si="0"/>
         <v>=ERF.PRECISE($A5)</v>
       </c>
-      <c r="D5" s="3">
-        <v>-0.99999925690162705</v>
-      </c>
+      <c r="D5" s="3"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
@@ -567,9 +554,7 @@
         <f t="shared" ca="1" si="0"/>
         <v>=ERF.PRECISE($A6)</v>
       </c>
-      <c r="D6" s="3">
-        <v>-0.99997790950300003</v>
-      </c>
+      <c r="D6" s="3"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
@@ -584,9 +569,7 @@
         <f ca="1">_xlfn.FORMULATEXT($B7)</f>
         <v>=ERF.PRECISE($A7)</v>
       </c>
-      <c r="D7" s="3">
-        <v>-0.99959304798255499</v>
-      </c>
+      <c r="D7" s="3"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
@@ -601,9 +584,7 @@
         <f t="shared" ref="C8:C22" ca="1" si="3">_xlfn.FORMULATEXT($B8)</f>
         <v>=ERF.PRECISE($A8)</v>
       </c>
-      <c r="D8" s="3">
-        <v>-0.99532226501895205</v>
-      </c>
+      <c r="D8" s="3"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
@@ -618,9 +599,7 @@
         <f t="shared" ca="1" si="3"/>
         <v>=ERF.PRECISE($A9)</v>
       </c>
-      <c r="D9" s="3">
-        <v>-0.96610514647530998</v>
-      </c>
+      <c r="D9" s="3"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
@@ -635,9 +614,7 @@
         <f t="shared" ca="1" si="3"/>
         <v>=ERF.PRECISE($A10)</v>
       </c>
-      <c r="D10" s="3">
-        <v>-0.84270079294971401</v>
-      </c>
+      <c r="D10" s="3"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
@@ -652,9 +629,7 @@
         <f t="shared" ca="1" si="3"/>
         <v>=ERF.PRECISE($A11)</v>
       </c>
-      <c r="D11" s="3">
-        <v>-0.52049987781304596</v>
-      </c>
+      <c r="D11" s="3"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
@@ -669,9 +644,7 @@
         <f t="shared" ca="1" si="3"/>
         <v>=ERF.PRECISE($A12)</v>
       </c>
-      <c r="D12" s="3">
-        <v>0</v>
-      </c>
+      <c r="D12" s="3"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
@@ -686,9 +659,7 @@
         <f t="shared" ca="1" si="3"/>
         <v>=ERF.PRECISE($A13)</v>
       </c>
-      <c r="D13" s="3">
-        <v>0.52049987781304596</v>
-      </c>
+      <c r="D13" s="3"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
@@ -703,9 +674,7 @@
         <f t="shared" ca="1" si="3"/>
         <v>=ERF.PRECISE($A14)</v>
       </c>
-      <c r="D14" s="3">
-        <v>0.84270079294971401</v>
-      </c>
+      <c r="D14" s="3"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
@@ -720,9 +689,7 @@
         <f t="shared" ca="1" si="3"/>
         <v>=ERF.PRECISE($A15)</v>
       </c>
-      <c r="D15" s="3">
-        <v>0.96610514647530998</v>
-      </c>
+      <c r="D15" s="3"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
@@ -737,9 +704,7 @@
         <f t="shared" ca="1" si="3"/>
         <v>=ERF.PRECISE($A16)</v>
       </c>
-      <c r="D16" s="3">
-        <v>0.99532226501895205</v>
-      </c>
+      <c r="D16" s="3"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
@@ -754,9 +719,7 @@
         <f t="shared" ca="1" si="3"/>
         <v>=ERF.PRECISE($A17)</v>
       </c>
-      <c r="D17" s="3">
-        <v>0.99959304798255499</v>
-      </c>
+      <c r="D17" s="3"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
@@ -771,9 +734,7 @@
         <f t="shared" ca="1" si="3"/>
         <v>=ERF.PRECISE($A18)</v>
       </c>
-      <c r="D18" s="3">
-        <v>0.99997790950300003</v>
-      </c>
+      <c r="D18" s="3"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
@@ -788,9 +749,7 @@
         <f t="shared" ca="1" si="3"/>
         <v>=ERF.PRECISE($A19)</v>
       </c>
-      <c r="D19" s="3">
-        <v>0.99999925690162705</v>
-      </c>
+      <c r="D19" s="3"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
@@ -805,9 +764,7 @@
         <f t="shared" ca="1" si="3"/>
         <v>=ERF.PRECISE($A20)</v>
       </c>
-      <c r="D20" s="3">
-        <v>0.99999998458274197</v>
-      </c>
+      <c r="D20" s="3"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
@@ -822,9 +779,7 @@
         <f t="shared" ca="1" si="3"/>
         <v>=ERF.PRECISE($A21)</v>
       </c>
-      <c r="D21" s="3">
-        <v>0.99999999980338306</v>
-      </c>
+      <c r="D21" s="3"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
@@ -839,9 +794,7 @@
         <f t="shared" ca="1" si="3"/>
         <v>=ERF.PRECISE($A22)</v>
       </c>
-      <c r="D22" s="3">
-        <v>0.99999999999846201</v>
-      </c>
+      <c r="D22" s="3"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
@@ -876,13 +829,13 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -895,7 +848,7 @@
         <v>=ERF.PRECISE(SQRT(-1))</v>
       </c>
       <c r="C29" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -908,7 +861,7 @@
         <v>=ERF.PRECISE("str")</v>
       </c>
       <c r="C30" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -921,7 +874,7 @@
         <v>=ERF.PRECISE(10/0)</v>
       </c>
       <c r="C31" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>